<commit_message>
Nouveau PHP, correction InfosPokemon, mise à jour script d'insertion + estimation
</commit_message>
<xml_diff>
--- a/estimation_TanyaVanier.xlsx
+++ b/estimation_TanyaVanier.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -360,6 +360,33 @@
   </si>
   <si>
     <t>Fière du travail accompli, même si je n'ai pas eu tout le temps voulu pour travailler sur mon projet. Le script d'insertion n'est donc pas fini, comme j'avais prévu initialement. J'ai terminé de remplir la plupart des tables, il me reste la table tblpokemonendroit qui est un gros morceau, ensuite ça devrait bien aller. Je suis particulièrement fière de cette itération parce que j'ai travaillé en continu sur mon projet à chaque moment possible.</t>
+  </si>
+  <si>
+    <t>08-04-2019</t>
+  </si>
+  <si>
+    <t>09-04-2019</t>
+  </si>
+  <si>
+    <t>10-04-2019</t>
+  </si>
+  <si>
+    <t>18-04-2019</t>
+  </si>
+  <si>
+    <t>Changer le ScrollView pour un RecyclerView (liste_pokemon)</t>
+  </si>
+  <si>
+    <t>24-04-2019</t>
+  </si>
+  <si>
+    <t>Changer le ScrollView pour un RecyclerView (liste_pokemon). Finalement, décider de garder le ScrollView et changer les filtres</t>
+  </si>
+  <si>
+    <t>25-04-2019</t>
+  </si>
+  <si>
+    <t>Changer les filtres de la liste_pokemon pour avoir moins de données à charger en même temps. Modifier quelques PHP (enlever les anciens pour les filtres et en mettre un nouveau), Corriger le PHP InfosPokemon</t>
   </si>
 </sst>
 </file>
@@ -2781,7 +2808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -3084,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3142,34 +3169,70 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
@@ -3263,7 +3326,7 @@
       <c r="B37" s="22"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>